<commit_message>
move hrex requirements into pas requirement set
</commit_message>
<xml_diff>
--- a/lib/davinci_pas_test_kit/requirements/hl7.fhir.us.davinci-pas_2.0.1_requirements.xlsx
+++ b/lib/davinci_pas_test_kit/requirements/hl7.fhir.us.davinci-pas_2.0.1_requirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstrassner/repo/inferno/davinci-pas-test-kit/lib/davinci_pas_test_kit/requirements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/knaden/Documents/Inferno/source/davinci-pas-test-kit/lib/davinci_pas_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F2BFA5-CC96-5147-B31D-6520D8749380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE072E9-5295-0B4D-9CFC-88C2A1595C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="3280" windowWidth="47560" windowHeight="20620" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20280" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="366">
   <si>
     <r>
       <rPr>
@@ -993,9 +993,6 @@
     <t>The HRex IG defines some [conformance expectations](http://hl7.org/fhir/us/davinci-hrex/conformance.html) that all Da Vinci IGs are expected to follow.</t>
   </si>
   <si>
-    <t>hl7.fhir.us.davinci-hrex_1.0.0@21-32</t>
-  </si>
-  <si>
     <t>PA Intermediary Systems **SHALL** be capable of processing all data elements that are marked as Must Support on the Claim Request</t>
   </si>
   <si>
@@ -1072,9 +1069,6 @@
   </si>
   <si>
     <t>[Servers] claiming conformance to this IG **SHALL** comply with the [Security and Privacy page in the Da Vinci HRex guide](http://hl7.org/fhir/us/davinci-hrex/security.html).</t>
-  </si>
-  <si>
-    <t>hl7.fhir.us.davinci-hrex_1.0.0@1-20</t>
   </si>
   <si>
     <t>[Clients] claiming conformance to this IG **SHALL** comply with the [Security and Privacy page in the Da Vinci HRex guide](http://hl7.org/fhir/us/davinci-hrex/security.html).</t>
@@ -2419,6 +2413,86 @@
       </rPr>
       <t>Mapping: none</t>
     </r>
+  </si>
+  <si>
+    <t>HRex security requirements are general and currently handled as attestation in other test kits, so not creating explicit subrequirements for this.</t>
+  </si>
+  <si>
+    <t>https://hl7.org/fhir/us/davinci-hrex/STU1/conformance.html</t>
+  </si>
+  <si>
+    <t>In the context of an HRex compliant IG, mustSupport on any data element **SHALL** be interpreted [to mean that] … Data Sources **SHALL** be capable of populating the data element when sharing resources compliant with the profile. I.e. the system must be able to demonstrate the population and sharing of the element</t>
+  </si>
+  <si>
+    <t>In the context of an HRex compliant IG, mustSupport on any data element **SHALL** be interpreted [to mean that] … it is acceptable to omit the [must support] element if the [data source] system doesn't have values in a particular instance.</t>
+  </si>
+  <si>
+    <t>If the source doesn't have data for the element</t>
+  </si>
+  <si>
+    <t>In the context of an HRex compliant IG, mustSupport on any data element **SHALL** be interpreted [to mean that] … Data Consumers **SHALL** be capable of processing resource instances containing the data elements without generating an error or causing the application to fail.</t>
+  </si>
+  <si>
+    <t>In the context of an HRex compliant IG, mustSupport on any data element **SHALL** be interpreted [to mean that] … [i]f the minimum cardinality of an element is greater than 0 – i.e. the element is ‘required’, then the element **SHALL** be present in the instance</t>
+  </si>
+  <si>
+    <t>If the minimum cardinality is &gt; 0</t>
+  </si>
+  <si>
+    <t>In the context of an HRex compliant IG, mustSupport on any data element **SHALL** be interpreted [to mean that] …  [i]f the minimum cardinality of an element is greater than 0 – i.e. the element is ‘required’, then the element ... **SHALL** have a value unless:
+- The profile explicitly declares the dataAbsentReason extension or other extension for the element, in which case an extension can be present in place of the value. [or]
+- The profile is inherited from U.S. Core, in which case a dataAbsentReason extension may be sent in place of the value even where dataAbsentReason is not explicitly declared in the profile.</t>
+  </si>
+  <si>
+    <t>In the context of an HRex compliant IG, mustSupport on any data element **SHALL** be interpreted [to mean that] … Data Consumers **SHALL** interpret missing data elements within resource instances as data not being present in the Data Source’s systems or was not deemed to be shareable with the Data Consumer for privacy or other business reasons.</t>
+  </si>
+  <si>
+    <t>If the element is missing</t>
+  </si>
+  <si>
+    <t>In the context of an HRex compliant IG, mustSupport on any data element **SHALL** be interpreted [to mean that] … [w]here the value set for an element includes concepts such as “unknown”, “refused to answer”, “not available” or where dataAbsentReason is explicitly referenced in a profile, then Data Sources **SHALL** use these values/that extension to communicate the reason for missing data.</t>
+  </si>
+  <si>
+    <t>When value sets include certain concepts</t>
+  </si>
+  <si>
+    <t>In the context of an HRex compliant IG, mustSupport on any data element **SHALL** be interpreted [to mean that] … Data Consumers **SHALL** be able to process resource instances containing data elements that have extensions in place of a value where such extensions are declared as part of the profile.</t>
+  </si>
+  <si>
+    <t>When extensions are used instead of a value</t>
+  </si>
+  <si>
+    <t>[Data sources] are free to include additional data [beyond the must support elements]</t>
+  </si>
+  <si>
+    <t>[R]eceivers **SHOULD NOT** reject instances that contain unexpected [non-must support] data elements if those elements are not [modifier elements](http://hl7.org/fhir/R4/conformance-rules.html#isModifier).</t>
+  </si>
+  <si>
+    <t>When non-must support elements present</t>
+  </si>
+  <si>
+    <t>[Data Sources] should be aware that they can't count on receivers storing, processing or doing anything other than ignoring data that is not marked as mustSupport.</t>
+  </si>
+  <si>
+    <t>When sending non must support elements</t>
+  </si>
+  <si>
+    <t>Can only be tested in the context of a specific trading partner</t>
+  </si>
+  <si>
+    <t>Many of the profiles in this guide reference other FHIR resources that are US Core profiles. This is defined in the formal profile definitions. For example, US Core Patient. For any other references not formally defined in a US Core profiles, the referenced resource **SHOULD** be a US Core profile if a US Core profile exists for the resource type.</t>
+  </si>
+  <si>
+    <t>When referencing US Core resource types</t>
+  </si>
+  <si>
+    <t>HRex not represented as a separate requirements set, so relevant requirements for PAS are included</t>
+  </si>
+  <si>
+    <t>hl7.fhir.us.davinci-pas_2.0.1@212,213,215,216,218,220,222,223</t>
+  </si>
+  <si>
+    <t>hl7.fhir.us.davinci-pas_2.0.1@214,217,219,221</t>
   </si>
 </sst>
 </file>
@@ -2818,7 +2892,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2931,6 +3005,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3269,7 +3349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6AA7094-ECFF-0B4E-A5C9-6F41B8D76EEB}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3301,7 +3381,7 @@
     </row>
     <row r="4" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="43" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B4" s="35"/>
       <c r="C4" s="36"/>
@@ -3354,11 +3434,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}">
   <dimension ref="A1:AI341"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="8" ySplit="1" topLeftCell="I34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4435,7 +4515,7 @@
         <v>74</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>30</v>
@@ -4455,7 +4535,7 @@
         <v/>
       </c>
       <c r="T31" s="16" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="51" x14ac:dyDescent="0.2">
@@ -4520,7 +4600,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="102" x14ac:dyDescent="0.2">
       <c r="A34" s="7">
         <v>33</v>
       </c>
@@ -4537,7 +4617,7 @@
         <v>30</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>79</v>
+        <v>364</v>
       </c>
       <c r="G34" s="7" t="b">
         <v>0</v>
@@ -4568,7 +4648,7 @@
         <v>37</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>79</v>
+        <v>365</v>
       </c>
       <c r="G35" s="7" t="b">
         <v>0</v>
@@ -4590,7 +4670,7 @@
         <v>77</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>29</v>
@@ -4618,7 +4698,7 @@
         <v>77</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>29</v>
@@ -4646,7 +4726,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>29</v>
@@ -4674,7 +4754,7 @@
         <v>77</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>29</v>
@@ -4702,7 +4782,7 @@
         <v>77</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>29</v>
@@ -4730,7 +4810,7 @@
         <v>77</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>29</v>
@@ -4758,10 +4838,10 @@
         <v>77</v>
       </c>
       <c r="C42" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>87</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>37</v>
@@ -4770,7 +4850,7 @@
         <v>1</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M42" s="9" t="str" cm="1">
         <f t="array" ref="M42">PAGE_NAME(B42)</f>
@@ -4789,7 +4869,7 @@
         <v>77</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>36</v>
@@ -4817,7 +4897,7 @@
         <v>77</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>44</v>
@@ -4829,7 +4909,7 @@
         <v>1</v>
       </c>
       <c r="H44" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M44" s="9" t="str" cm="1">
         <f t="array" ref="M44">PAGE_NAME(B44)</f>
@@ -4845,10 +4925,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>93</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>29</v>
@@ -4873,10 +4953,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>29</v>
@@ -4901,10 +4981,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>29</v>
@@ -4929,10 +5009,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>29</v>
@@ -4952,15 +5032,15 @@
         <v>integration-with-other-implementation-guides</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
         <v>48</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>29</v>
@@ -4980,15 +5060,15 @@
         <v>integration-with-other-implementation-guides</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="7">
         <v>49</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>29</v>
@@ -5008,15 +5088,15 @@
         <v>integration-with-other-implementation-guides</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
         <v>50</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>47</v>
@@ -5036,15 +5116,15 @@
         <v>integration-with-other-implementation-guides</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A52" s="7">
         <v>51</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>47</v>
@@ -5064,15 +5144,15 @@
         <v>integration-with-other-implementation-guides</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A53" s="7">
         <v>52</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>47</v>
@@ -5092,15 +5172,15 @@
         <v>integration-with-other-implementation-guides</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A54" s="7">
         <v>53</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>47</v>
@@ -5120,15 +5200,15 @@
         <v>integration-with-other-implementation-guides</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>54</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>47</v>
@@ -5148,15 +5228,15 @@
         <v>integration-with-other-implementation-guides</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <v>55</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>47</v>
@@ -5176,24 +5256,21 @@
         <v>integration-with-other-implementation-guides</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <v>56</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>29</v>
       </c>
       <c r="E57" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="F57" s="8" t="s">
-        <v>106</v>
       </c>
       <c r="G57" s="7" t="b">
         <v>0</v>
@@ -5206,25 +5283,25 @@
         <f t="array" ref="N57">SECTION_NAME(B57)</f>
         <v>integration-with-other-implementation-guides</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="T57" s="16" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" ht="85" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
         <v>57</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>29</v>
       </c>
       <c r="E58" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="F58" s="8" t="s">
-        <v>106</v>
       </c>
       <c r="G58" s="7" t="b">
         <v>0</v>
@@ -5237,16 +5314,19 @@
         <f t="array" ref="N58">SECTION_NAME(B58)</f>
         <v>integration-with-other-implementation-guides</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="T58" s="16" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>58</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>29</v>
@@ -5266,15 +5346,15 @@
         <v>summary</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" ht="102" x14ac:dyDescent="0.2">
       <c r="A60" s="7">
         <v>59</v>
       </c>
       <c r="B60" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C60" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>110</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>29</v>
@@ -5294,15 +5374,15 @@
         <v>summary</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" ht="136" x14ac:dyDescent="0.2">
       <c r="A61" s="7">
         <v>60</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>29</v>
@@ -5322,15 +5402,15 @@
         <v>summary</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="153" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" ht="153" x14ac:dyDescent="0.2">
       <c r="A62" s="7">
         <v>61</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>29</v>
@@ -5350,15 +5430,15 @@
         <v>summary</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" ht="136" x14ac:dyDescent="0.2">
       <c r="A63" s="7">
         <v>62</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>29</v>
@@ -5378,15 +5458,15 @@
         <v>summary</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" ht="119" x14ac:dyDescent="0.2">
       <c r="A64" s="7">
         <v>63</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>29</v>
@@ -5411,10 +5491,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>29</v>
@@ -5439,10 +5519,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>47</v>
@@ -5467,10 +5547,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D67" s="7" t="s">
         <v>29</v>
@@ -5482,7 +5562,7 @@
         <v>1</v>
       </c>
       <c r="H67" s="16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M67" s="9" t="str" cm="1">
         <f t="array" ref="M67">PAGE_NAME(B67)</f>
@@ -5498,10 +5578,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>29</v>
@@ -5513,7 +5593,7 @@
         <v>1</v>
       </c>
       <c r="H68" s="16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M68" s="9" t="str" cm="1">
         <f t="array" ref="M68">PAGE_NAME(B68)</f>
@@ -5529,10 +5609,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D69" s="7" t="s">
         <v>44</v>
@@ -5544,7 +5624,7 @@
         <v>1</v>
       </c>
       <c r="H69" s="16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M69" s="9" t="str" cm="1">
         <f t="array" ref="M69">PAGE_NAME(B69)</f>
@@ -5560,10 +5640,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>44</v>
@@ -5575,7 +5655,7 @@
         <v>1</v>
       </c>
       <c r="H70" s="16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M70" s="9" t="str" cm="1">
         <f t="array" ref="M70">PAGE_NAME(B70)</f>
@@ -5591,10 +5671,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D71" s="7" t="s">
         <v>29</v>
@@ -5619,10 +5699,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C72" s="8" t="s">
         <v>122</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>124</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>29</v>
@@ -5647,10 +5727,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>29</v>
@@ -5675,10 +5755,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>44</v>
@@ -5703,10 +5783,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>29</v>
@@ -5731,10 +5811,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>29</v>
@@ -5759,10 +5839,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D77" s="7" t="s">
         <v>29</v>
@@ -5787,10 +5867,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>29</v>
@@ -5802,7 +5882,7 @@
         <v>1</v>
       </c>
       <c r="H78" s="16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M78" s="9" t="str" cm="1">
         <f t="array" ref="M78">PAGE_NAME(B78)</f>
@@ -5818,10 +5898,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D79" s="7" t="s">
         <v>29</v>
@@ -5846,10 +5926,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>29</v>
@@ -5874,10 +5954,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>29</v>
@@ -5902,10 +5982,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D82" s="7" t="s">
         <v>29</v>
@@ -5930,10 +6010,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D83" s="7" t="s">
         <v>29</v>
@@ -5958,10 +6038,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>29</v>
@@ -5986,10 +6066,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>47</v>
@@ -6014,10 +6094,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D86" s="7" t="s">
         <v>29</v>
@@ -6042,10 +6122,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D87" s="7" t="s">
         <v>29</v>
@@ -6070,10 +6150,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D88" s="7" t="s">
         <v>44</v>
@@ -6098,10 +6178,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D89" s="7" t="s">
         <v>47</v>
@@ -6113,7 +6193,7 @@
         <v>1</v>
       </c>
       <c r="H89" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M89" s="9" t="str" cm="1">
         <f t="array" ref="M89">PAGE_NAME(B89)</f>
@@ -6129,10 +6209,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D90" s="7" t="s">
         <v>29</v>
@@ -6144,7 +6224,7 @@
         <v>1</v>
       </c>
       <c r="H90" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M90" s="9" t="str" cm="1">
         <f t="array" ref="M90">PAGE_NAME(B90)</f>
@@ -6160,10 +6240,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D91" s="7" t="s">
         <v>44</v>
@@ -6175,7 +6255,7 @@
         <v>1</v>
       </c>
       <c r="H91" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M91" s="9" t="str" cm="1">
         <f t="array" ref="M91">PAGE_NAME(B91)</f>
@@ -6191,10 +6271,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D92" s="7" t="s">
         <v>29</v>
@@ -6219,10 +6299,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D93" s="7" t="s">
         <v>29</v>
@@ -6247,10 +6327,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D94" s="7" t="s">
         <v>29</v>
@@ -6275,10 +6355,10 @@
         <v>94</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D95" s="7" t="s">
         <v>44</v>
@@ -6303,10 +6383,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D96" s="7" t="s">
         <v>29</v>
@@ -6318,7 +6398,7 @@
         <v>1</v>
       </c>
       <c r="H96" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M96" s="9" t="str" cm="1">
         <f t="array" ref="M96">PAGE_NAME(B96)</f>
@@ -6334,10 +6414,10 @@
         <v>96</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D97" s="7" t="s">
         <v>29</v>
@@ -6350,7 +6430,7 @@
         <v>1</v>
       </c>
       <c r="H97" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="I97" s="30" t="s">
         <v>54</v>
@@ -6375,10 +6455,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D98" s="7" t="s">
         <v>29</v>
@@ -6390,7 +6470,7 @@
         <v>1</v>
       </c>
       <c r="H98" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="M98" s="9" t="str" cm="1">
         <f t="array" ref="M98">PAGE_NAME(B98)</f>
@@ -6406,10 +6486,10 @@
         <v>98</v>
       </c>
       <c r="B99" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D99" s="7" t="s">
         <v>29</v>
@@ -6434,10 +6514,10 @@
         <v>99</v>
       </c>
       <c r="B100" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D100" s="7" t="s">
         <v>29</v>
@@ -6462,10 +6542,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C101" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="C101" s="8" t="s">
-        <v>158</v>
       </c>
       <c r="D101" s="7" t="s">
         <v>29</v>
@@ -6490,10 +6570,10 @@
         <v>101</v>
       </c>
       <c r="B102" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D102" s="7" t="s">
         <v>29</v>
@@ -6518,10 +6598,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D103" s="7" t="s">
         <v>29</v>
@@ -6533,7 +6613,7 @@
         <v>1</v>
       </c>
       <c r="H103" s="16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="M103" s="9" t="str" cm="1">
         <f t="array" ref="M103">PAGE_NAME(B103)</f>
@@ -6549,10 +6629,10 @@
         <v>103</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D104" s="7" t="s">
         <v>29</v>
@@ -6564,7 +6644,7 @@
         <v>1</v>
       </c>
       <c r="H104" s="16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M104" s="9" t="str" cm="1">
         <f t="array" ref="M104">PAGE_NAME(B104)</f>
@@ -6580,10 +6660,10 @@
         <v>104</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D105" s="7" t="s">
         <v>29</v>
@@ -6595,7 +6675,7 @@
         <v>1</v>
       </c>
       <c r="H105" s="16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="M105" s="9" t="str" cm="1">
         <f t="array" ref="M105">PAGE_NAME(B105)</f>
@@ -6611,10 +6691,10 @@
         <v>105</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D106" s="7" t="s">
         <v>29</v>
@@ -6626,7 +6706,7 @@
         <v>1</v>
       </c>
       <c r="H106" s="16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="M106" s="9" t="str" cm="1">
         <f t="array" ref="M106">PAGE_NAME(B106)</f>
@@ -6642,13 +6722,13 @@
         <v>106</v>
       </c>
       <c r="B107" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E107" s="7" t="s">
         <v>30</v>
@@ -6657,7 +6737,7 @@
         <v>1</v>
       </c>
       <c r="H107" s="16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="M107" s="9" t="str" cm="1">
         <f t="array" ref="M107">PAGE_NAME(B107)</f>
@@ -6673,10 +6753,10 @@
         <v>107</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D108" s="7" t="s">
         <v>29</v>
@@ -6701,10 +6781,10 @@
         <v>108</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D109" s="7" t="s">
         <v>47</v>
@@ -6719,7 +6799,7 @@
         <v>55</v>
       </c>
       <c r="J109" s="30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K109" s="30" t="s">
         <v>55</v>
@@ -6738,10 +6818,10 @@
         <v>109</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D110" s="7" t="s">
         <v>47</v>
@@ -6756,7 +6836,7 @@
         <v>55</v>
       </c>
       <c r="J110" s="30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K110" s="30" t="s">
         <v>55</v>
@@ -6775,10 +6855,10 @@
         <v>110</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D111" s="7" t="s">
         <v>29</v>
@@ -6803,10 +6883,10 @@
         <v>111</v>
       </c>
       <c r="B112" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D112" s="7" t="s">
         <v>29</v>
@@ -6818,7 +6898,7 @@
         <v>1</v>
       </c>
       <c r="H112" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="M112" s="9" t="str" cm="1">
         <f t="array" ref="M112">PAGE_NAME(B112)</f>
@@ -6834,10 +6914,10 @@
         <v>112</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D113" s="7" t="s">
         <v>29</v>
@@ -6849,7 +6929,7 @@
         <v>1</v>
       </c>
       <c r="H113" s="16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="M113" s="9" t="str" cm="1">
         <f t="array" ref="M113">PAGE_NAME(B113)</f>
@@ -6865,10 +6945,10 @@
         <v>113</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D114" s="7" t="s">
         <v>29</v>
@@ -6880,7 +6960,7 @@
         <v>1</v>
       </c>
       <c r="H114" s="16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="115" spans="1:20" ht="102" x14ac:dyDescent="0.2">
@@ -6888,10 +6968,10 @@
         <v>114</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D115" s="7" t="s">
         <v>29</v>
@@ -6903,7 +6983,7 @@
         <v>1</v>
       </c>
       <c r="H115" s="16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="M115" s="9" t="str" cm="1">
         <f t="array" ref="M115">PAGE_NAME(B115)</f>
@@ -6919,10 +6999,10 @@
         <v>115</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D116" s="7" t="s">
         <v>29</v>
@@ -6934,7 +7014,7 @@
         <v>1</v>
       </c>
       <c r="H116" s="16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="M116" s="9" t="str" cm="1">
         <f t="array" ref="M116">PAGE_NAME(B116)</f>
@@ -6950,10 +7030,10 @@
         <v>116</v>
       </c>
       <c r="B117" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D117" s="7" t="s">
         <v>44</v>
@@ -6965,7 +7045,7 @@
         <v>1</v>
       </c>
       <c r="H117" s="16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M117" s="9" t="str" cm="1">
         <f t="array" ref="M117">PAGE_NAME(B117)</f>
@@ -6981,10 +7061,10 @@
         <v>117</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D118" s="7" t="s">
         <v>47</v>
@@ -6996,7 +7076,7 @@
         <v>1</v>
       </c>
       <c r="H118" s="16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M118" s="9" t="str" cm="1">
         <f t="array" ref="M118">PAGE_NAME(B118)</f>
@@ -7012,13 +7092,13 @@
         <v>118</v>
       </c>
       <c r="B119" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C119" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D119" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="C119" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="D119" s="7" t="s">
-        <v>188</v>
       </c>
       <c r="M119" s="9" t="str" cm="1">
         <f t="array" ref="M119">PAGE_NAME(B119)</f>
@@ -7029,7 +7109,7 @@
         <v>prior-authorization-workflow-diagrams</v>
       </c>
       <c r="T119" s="16" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="120" spans="1:20" ht="85" x14ac:dyDescent="0.2">
@@ -7037,10 +7117,10 @@
         <v>119</v>
       </c>
       <c r="B120" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D120" s="7" t="s">
         <v>29</v>
@@ -7065,10 +7145,10 @@
         <v>120</v>
       </c>
       <c r="B121" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="C121" s="8" t="s">
         <v>189</v>
-      </c>
-      <c r="C121" s="8" t="s">
-        <v>191</v>
       </c>
       <c r="D121" s="7" t="s">
         <v>29</v>
@@ -7080,7 +7160,7 @@
         <v>1</v>
       </c>
       <c r="H121" s="16" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M121" s="9" t="str" cm="1">
         <f t="array" ref="M121">PAGE_NAME(B121)</f>
@@ -7096,10 +7176,10 @@
         <v>121</v>
       </c>
       <c r="B122" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D122" s="7" t="s">
         <v>29</v>
@@ -7124,10 +7204,10 @@
         <v>122</v>
       </c>
       <c r="B123" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D123" s="7" t="s">
         <v>29</v>
@@ -7152,10 +7232,10 @@
         <v>123</v>
       </c>
       <c r="B124" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D124" s="7" t="s">
         <v>29</v>
@@ -7185,10 +7265,10 @@
         <v>124</v>
       </c>
       <c r="B125" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D125" s="7" t="s">
         <v>29</v>
@@ -7206,7 +7286,7 @@
         <v>55</v>
       </c>
       <c r="L125" s="30" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M125" s="9" t="str" cm="1">
         <f t="array" ref="M125">PAGE_NAME(B125)</f>
@@ -7222,10 +7302,10 @@
         <v>125</v>
       </c>
       <c r="B126" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D126" s="7" t="s">
         <v>29</v>
@@ -7250,10 +7330,10 @@
         <v>126</v>
       </c>
       <c r="B127" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D127" s="7" t="s">
         <v>29</v>
@@ -7278,10 +7358,10 @@
         <v>127</v>
       </c>
       <c r="B128" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D128" s="7" t="s">
         <v>29</v>
@@ -7306,13 +7386,13 @@
         <v>128</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D129" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E129" s="7" t="s">
         <v>37</v>
@@ -7334,10 +7414,10 @@
         <v>129</v>
       </c>
       <c r="B130" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D130" s="7" t="s">
         <v>29</v>
@@ -7362,10 +7442,10 @@
         <v>130</v>
       </c>
       <c r="B131" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D131" s="7" t="s">
         <v>29</v>
@@ -7390,10 +7470,10 @@
         <v>131</v>
       </c>
       <c r="B132" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D132" s="7" t="s">
         <v>29</v>
@@ -7418,10 +7498,10 @@
         <v>132</v>
       </c>
       <c r="B133" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D133" s="7" t="s">
         <v>29</v>
@@ -7433,7 +7513,7 @@
         <v>1</v>
       </c>
       <c r="H133" s="16" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I133" s="30" t="s">
         <v>54</v>
@@ -7442,7 +7522,7 @@
         <v>55</v>
       </c>
       <c r="L133" s="30" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M133" s="9" t="str" cm="1">
         <f t="array" ref="M133">PAGE_NAME(B133)</f>
@@ -7458,10 +7538,10 @@
         <v>133</v>
       </c>
       <c r="B134" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D134" s="7" t="s">
         <v>29</v>
@@ -7473,7 +7553,7 @@
         <v>1</v>
       </c>
       <c r="H134" s="16" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="M134" s="9" t="str" cm="1">
         <f t="array" ref="M134">PAGE_NAME(B134)</f>
@@ -7484,7 +7564,7 @@
         <v>prior-authorization-inquiries</v>
       </c>
       <c r="T134" s="16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="135" spans="1:20" ht="136" x14ac:dyDescent="0.2">
@@ -7492,10 +7572,10 @@
         <v>134</v>
       </c>
       <c r="B135" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D135" s="7" t="s">
         <v>44</v>
@@ -7507,7 +7587,7 @@
         <v>1</v>
       </c>
       <c r="H135" s="16" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M135" s="9" t="str" cm="1">
         <f t="array" ref="M135">PAGE_NAME(B135)</f>
@@ -7523,10 +7603,10 @@
         <v>135</v>
       </c>
       <c r="B136" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D136" s="7" t="s">
         <v>47</v>
@@ -7538,7 +7618,7 @@
         <v>1</v>
       </c>
       <c r="H136" s="16" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="M136" s="9" t="str" cm="1">
         <f t="array" ref="M136">PAGE_NAME(B136)</f>
@@ -7554,10 +7634,10 @@
         <v>136</v>
       </c>
       <c r="B137" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D137" s="7" t="s">
         <v>29</v>
@@ -7569,7 +7649,7 @@
         <v>1</v>
       </c>
       <c r="H137" s="16" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="M137" s="9" t="str" cm="1">
         <f t="array" ref="M137">PAGE_NAME(B137)</f>
@@ -7585,10 +7665,10 @@
         <v>137</v>
       </c>
       <c r="B138" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D138" s="7" t="s">
         <v>29</v>
@@ -7613,10 +7693,10 @@
         <v>138</v>
       </c>
       <c r="B139" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D139" s="7" t="s">
         <v>29</v>
@@ -7641,10 +7721,10 @@
         <v>139</v>
       </c>
       <c r="B140" s="11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D140" s="7" t="s">
         <v>29</v>
@@ -7656,7 +7736,7 @@
         <v>1</v>
       </c>
       <c r="H140" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M140" s="9" t="str" cm="1">
         <f t="array" ref="M140">PAGE_NAME(B140)</f>
@@ -7672,10 +7752,10 @@
         <v>140</v>
       </c>
       <c r="B141" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D141" s="7" t="s">
         <v>29</v>
@@ -7700,10 +7780,10 @@
         <v>141</v>
       </c>
       <c r="B142" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="C142" s="8" t="s">
         <v>222</v>
-      </c>
-      <c r="C142" s="8" t="s">
-        <v>224</v>
       </c>
       <c r="D142" s="7" t="s">
         <v>29</v>
@@ -7728,10 +7808,10 @@
         <v>142</v>
       </c>
       <c r="B143" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D143" s="7" t="s">
         <v>29</v>
@@ -7756,10 +7836,10 @@
         <v>143</v>
       </c>
       <c r="B144" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D144" s="7" t="s">
         <v>29</v>
@@ -7784,10 +7864,10 @@
         <v>144</v>
       </c>
       <c r="B145" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D145" s="7" t="s">
         <v>29</v>
@@ -7812,10 +7892,10 @@
         <v>145</v>
       </c>
       <c r="B146" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D146" s="7" t="s">
         <v>29</v>
@@ -7840,10 +7920,10 @@
         <v>146</v>
       </c>
       <c r="B147" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C147" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D147" s="7" t="s">
         <v>44</v>
@@ -7868,10 +7948,10 @@
         <v>147</v>
       </c>
       <c r="B148" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D148" s="7" t="s">
         <v>44</v>
@@ -7896,10 +7976,10 @@
         <v>148</v>
       </c>
       <c r="B149" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C149" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D149" s="7" t="s">
         <v>29</v>
@@ -7924,10 +8004,10 @@
         <v>149</v>
       </c>
       <c r="B150" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C150" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D150" s="7" t="s">
         <v>29</v>
@@ -7952,10 +8032,10 @@
         <v>150</v>
       </c>
       <c r="B151" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C151" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D151" s="7" t="s">
         <v>47</v>
@@ -7980,10 +8060,10 @@
         <v>151</v>
       </c>
       <c r="B152" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C152" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D152" s="7" t="s">
         <v>44</v>
@@ -8008,10 +8088,10 @@
         <v>152</v>
       </c>
       <c r="B153" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C153" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D153" s="7" t="s">
         <v>29</v>
@@ -8036,10 +8116,10 @@
         <v>153</v>
       </c>
       <c r="B154" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C154" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D154" s="7" t="s">
         <v>29</v>
@@ -8064,10 +8144,10 @@
         <v>154</v>
       </c>
       <c r="B155" s="11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C155" s="8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D155" s="7" t="s">
         <v>44</v>
@@ -8092,10 +8172,10 @@
         <v>155</v>
       </c>
       <c r="B156" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="C156" s="8" t="s">
         <v>237</v>
-      </c>
-      <c r="C156" s="8" t="s">
-        <v>239</v>
       </c>
       <c r="D156" s="7" t="s">
         <v>29</v>
@@ -8120,10 +8200,10 @@
         <v>156</v>
       </c>
       <c r="B157" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C157" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D157" s="7" t="s">
         <v>47</v>
@@ -8148,10 +8228,10 @@
         <v>157</v>
       </c>
       <c r="B158" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="C158" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="C158" s="8" t="s">
-        <v>242</v>
       </c>
       <c r="D158" s="7" t="s">
         <v>44</v>
@@ -8163,7 +8243,7 @@
         <v>1</v>
       </c>
       <c r="H158" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M158" s="9" t="str" cm="1">
         <f t="array" ref="M158">PAGE_NAME(B158)</f>
@@ -8179,10 +8259,10 @@
         <v>158</v>
       </c>
       <c r="B159" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C159" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D159" s="7" t="s">
         <v>44</v>
@@ -8194,7 +8274,7 @@
         <v>1</v>
       </c>
       <c r="H159" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M159" s="9" t="str" cm="1">
         <f t="array" ref="M159">PAGE_NAME(B159)</f>
@@ -8210,10 +8290,10 @@
         <v>159</v>
       </c>
       <c r="B160" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C160" s="8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D160" s="7" t="s">
         <v>29</v>
@@ -8225,7 +8305,7 @@
         <v>1</v>
       </c>
       <c r="H160" s="16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="161" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -8233,10 +8313,10 @@
         <v>160</v>
       </c>
       <c r="B161" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C161" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D161" s="7" t="s">
         <v>44</v>
@@ -8248,7 +8328,7 @@
         <v>1</v>
       </c>
       <c r="H161" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M161" s="9" t="str" cm="1">
         <f t="array" ref="M161">PAGE_NAME(B161)</f>
@@ -8264,10 +8344,10 @@
         <v>161</v>
       </c>
       <c r="B162" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C162" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D162" s="7" t="s">
         <v>44</v>
@@ -8279,7 +8359,7 @@
         <v>1</v>
       </c>
       <c r="H162" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="163" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -8287,10 +8367,10 @@
         <v>162</v>
       </c>
       <c r="B163" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C163" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D163" s="7" t="s">
         <v>44</v>
@@ -8302,7 +8382,7 @@
         <v>1</v>
       </c>
       <c r="H163" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="164" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -8310,10 +8390,10 @@
         <v>163</v>
       </c>
       <c r="B164" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C164" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D164" s="7" t="s">
         <v>44</v>
@@ -8325,7 +8405,7 @@
         <v>1</v>
       </c>
       <c r="H164" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="165" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -8333,10 +8413,10 @@
         <v>164</v>
       </c>
       <c r="B165" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C165" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D165" s="7" t="s">
         <v>29</v>
@@ -8348,7 +8428,7 @@
         <v>1</v>
       </c>
       <c r="H165" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="166" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -8356,10 +8436,10 @@
         <v>165</v>
       </c>
       <c r="B166" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C166" s="8" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D166" s="7" t="s">
         <v>44</v>
@@ -8371,7 +8451,7 @@
         <v>1</v>
       </c>
       <c r="H166" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M166" s="9" t="str" cm="1">
         <f t="array" ref="M166">PAGE_NAME(B166)</f>
@@ -8387,10 +8467,10 @@
         <v>166</v>
       </c>
       <c r="B167" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C167" s="8" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D167" s="7" t="s">
         <v>29</v>
@@ -8402,7 +8482,7 @@
         <v>1</v>
       </c>
       <c r="H167" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M167" s="9" t="str" cm="1">
         <f t="array" ref="M167">PAGE_NAME(B167)</f>
@@ -8418,10 +8498,10 @@
         <v>167</v>
       </c>
       <c r="B168" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D168" s="7" t="s">
         <v>29</v>
@@ -8433,7 +8513,7 @@
         <v>1</v>
       </c>
       <c r="H168" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M168" s="9" t="str" cm="1">
         <f t="array" ref="M168">PAGE_NAME(B168)</f>
@@ -8449,10 +8529,10 @@
         <v>168</v>
       </c>
       <c r="B169" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D169" s="7" t="s">
         <v>29</v>
@@ -8464,7 +8544,7 @@
         <v>1</v>
       </c>
       <c r="H169" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M169" s="9" t="str" cm="1">
         <f t="array" ref="M169">PAGE_NAME(B169)</f>
@@ -8480,10 +8560,10 @@
         <v>169</v>
       </c>
       <c r="B170" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C170" s="8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D170" s="7" t="s">
         <v>29</v>
@@ -8495,7 +8575,7 @@
         <v>1</v>
       </c>
       <c r="H170" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M170" s="9" t="str" cm="1">
         <f t="array" ref="M170">PAGE_NAME(B170)</f>
@@ -8511,10 +8591,10 @@
         <v>170</v>
       </c>
       <c r="B171" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C171" s="8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D171" s="7" t="s">
         <v>29</v>
@@ -8526,7 +8606,7 @@
         <v>1</v>
       </c>
       <c r="H171" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M171" s="9" t="str" cm="1">
         <f t="array" ref="M171">PAGE_NAME(B171)</f>
@@ -8542,10 +8622,10 @@
         <v>171</v>
       </c>
       <c r="B172" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C172" s="8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D172" s="7" t="s">
         <v>29</v>
@@ -8557,7 +8637,7 @@
         <v>1</v>
       </c>
       <c r="H172" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M172" s="9" t="str" cm="1">
         <f t="array" ref="M172">PAGE_NAME(B172)</f>
@@ -8573,10 +8653,10 @@
         <v>172</v>
       </c>
       <c r="B173" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C173" s="8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D173" s="7" t="s">
         <v>29</v>
@@ -8588,7 +8668,7 @@
         <v>1</v>
       </c>
       <c r="H173" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M173" s="9" t="str" cm="1">
         <f t="array" ref="M173">PAGE_NAME(B173)</f>
@@ -8604,10 +8684,10 @@
         <v>173</v>
       </c>
       <c r="B174" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C174" s="8" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D174" s="7" t="s">
         <v>29</v>
@@ -8619,7 +8699,7 @@
         <v>1</v>
       </c>
       <c r="H174" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M174" s="9" t="str" cm="1">
         <f t="array" ref="M174">PAGE_NAME(B174)</f>
@@ -8635,10 +8715,10 @@
         <v>174</v>
       </c>
       <c r="B175" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C175" s="8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D175" s="7" t="s">
         <v>29</v>
@@ -8650,7 +8730,7 @@
         <v>1</v>
       </c>
       <c r="H175" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M175" s="9" t="str" cm="1">
         <f t="array" ref="M175">PAGE_NAME(B175)</f>
@@ -8666,10 +8746,10 @@
         <v>175</v>
       </c>
       <c r="B176" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C176" s="8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D176" s="7" t="s">
         <v>29</v>
@@ -8681,7 +8761,7 @@
         <v>1</v>
       </c>
       <c r="H176" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M176" s="9" t="str" cm="1">
         <f t="array" ref="M176">PAGE_NAME(B176)</f>
@@ -8697,10 +8777,10 @@
         <v>176</v>
       </c>
       <c r="B177" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C177" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D177" s="7" t="s">
         <v>29</v>
@@ -8712,7 +8792,7 @@
         <v>1</v>
       </c>
       <c r="H177" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M177" s="9" t="str" cm="1">
         <f t="array" ref="M177">PAGE_NAME(B177)</f>
@@ -8728,10 +8808,10 @@
         <v>177</v>
       </c>
       <c r="B178" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C178" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D178" s="7" t="s">
         <v>29</v>
@@ -8743,7 +8823,7 @@
         <v>1</v>
       </c>
       <c r="H178" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M178" s="9" t="str" cm="1">
         <f t="array" ref="M178">PAGE_NAME(B178)</f>
@@ -8759,10 +8839,10 @@
         <v>178</v>
       </c>
       <c r="B179" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C179" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D179" s="7" t="s">
         <v>44</v>
@@ -8774,7 +8854,7 @@
         <v>1</v>
       </c>
       <c r="H179" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M179" s="9" t="str" cm="1">
         <f t="array" ref="M179">PAGE_NAME(B179)</f>
@@ -8790,10 +8870,10 @@
         <v>179</v>
       </c>
       <c r="B180" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="C180" s="8" t="s">
         <v>265</v>
-      </c>
-      <c r="C180" s="8" t="s">
-        <v>267</v>
       </c>
       <c r="D180" s="7" t="s">
         <v>44</v>
@@ -8805,7 +8885,7 @@
         <v>1</v>
       </c>
       <c r="H180" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M180" s="9" t="str" cm="1">
         <f t="array" ref="M180">PAGE_NAME(B180)</f>
@@ -8821,10 +8901,10 @@
         <v>180</v>
       </c>
       <c r="B181" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D181" s="7" t="s">
         <v>29</v>
@@ -8836,7 +8916,7 @@
         <v>1</v>
       </c>
       <c r="H181" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M181" s="9" t="str" cm="1">
         <f t="array" ref="M181">PAGE_NAME(B181)</f>
@@ -8852,10 +8932,10 @@
         <v>181</v>
       </c>
       <c r="B182" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D182" s="7" t="s">
         <v>29</v>
@@ -8867,7 +8947,7 @@
         <v>1</v>
       </c>
       <c r="H182" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M182" s="9" t="str" cm="1">
         <f t="array" ref="M182">PAGE_NAME(B182)</f>
@@ -8883,10 +8963,10 @@
         <v>182</v>
       </c>
       <c r="B183" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C183" s="8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D183" s="7" t="s">
         <v>29</v>
@@ -8898,7 +8978,7 @@
         <v>1</v>
       </c>
       <c r="H183" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M183" s="9" t="str" cm="1">
         <f t="array" ref="M183">PAGE_NAME(B183)</f>
@@ -8914,10 +8994,10 @@
         <v>183</v>
       </c>
       <c r="B184" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C184" s="8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D184" s="7" t="s">
         <v>29</v>
@@ -8929,7 +9009,7 @@
         <v>1</v>
       </c>
       <c r="H184" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M184" s="9" t="str" cm="1">
         <f t="array" ref="M184">PAGE_NAME(B184)</f>
@@ -8945,10 +9025,10 @@
         <v>184</v>
       </c>
       <c r="B185" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C185" s="8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D185" s="7" t="s">
         <v>29</v>
@@ -8973,10 +9053,10 @@
         <v>185</v>
       </c>
       <c r="B186" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C186" s="8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D186" s="7" t="s">
         <v>29</v>
@@ -9001,10 +9081,10 @@
         <v>186</v>
       </c>
       <c r="B187" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C187" s="8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D187" s="7" t="s">
         <v>29</v>
@@ -9029,10 +9109,10 @@
         <v>187</v>
       </c>
       <c r="B188" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="C188" s="8" t="s">
         <v>274</v>
-      </c>
-      <c r="C188" s="8" t="s">
-        <v>276</v>
       </c>
       <c r="D188" s="7" t="s">
         <v>29</v>
@@ -9057,13 +9137,13 @@
         <v>188</v>
       </c>
       <c r="B189" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C189" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D189" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E189" s="7" t="s">
         <v>37</v>
@@ -9085,10 +9165,10 @@
         <v>189</v>
       </c>
       <c r="B190" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C190" s="8" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D190" s="7" t="s">
         <v>29</v>
@@ -9113,10 +9193,10 @@
         <v>190</v>
       </c>
       <c r="B191" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C191" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D191" s="7" t="s">
         <v>29</v>
@@ -9141,10 +9221,10 @@
         <v>191</v>
       </c>
       <c r="B192" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C192" s="8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D192" s="7" t="s">
         <v>47</v>
@@ -9156,7 +9236,7 @@
         <v>1</v>
       </c>
       <c r="H192" s="16" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I192" s="30" t="s">
         <v>54</v>
@@ -9165,7 +9245,7 @@
         <v>55</v>
       </c>
       <c r="L192" s="30" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M192" s="9" t="str" cm="1">
         <f t="array" ref="M192">PAGE_NAME(B192)</f>
@@ -9181,10 +9261,10 @@
         <v>192</v>
       </c>
       <c r="B193" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C193" s="8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D193" s="7" t="s">
         <v>47</v>
@@ -9209,10 +9289,10 @@
         <v>193</v>
       </c>
       <c r="B194" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C194" s="8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D194" s="7" t="s">
         <v>44</v>
@@ -9237,10 +9317,10 @@
         <v>194</v>
       </c>
       <c r="B195" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C195" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D195" s="7" t="s">
         <v>29</v>
@@ -9265,10 +9345,10 @@
         <v>195</v>
       </c>
       <c r="B196" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C196" s="8" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D196" s="7" t="s">
         <v>29</v>
@@ -9293,10 +9373,10 @@
         <v>196</v>
       </c>
       <c r="B197" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C197" s="8" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D197" s="7" t="s">
         <v>29</v>
@@ -9321,10 +9401,10 @@
         <v>197</v>
       </c>
       <c r="B198" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C198" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D198" s="7" t="s">
         <v>29</v>
@@ -9349,10 +9429,10 @@
         <v>198</v>
       </c>
       <c r="B199" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C199" s="8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D199" s="7" t="s">
         <v>29</v>
@@ -9377,10 +9457,10 @@
         <v>199</v>
       </c>
       <c r="B200" s="11" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C200" s="8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D200" s="7" t="s">
         <v>29</v>
@@ -9392,7 +9472,7 @@
         <v>0</v>
       </c>
       <c r="H200" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M200" s="9" t="str" cm="1">
         <f t="array" ref="M200">PAGE_NAME(B200)</f>
@@ -9408,10 +9488,10 @@
         <v>200</v>
       </c>
       <c r="B201" s="11" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C201" s="8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D201" s="7" t="s">
         <v>29</v>
@@ -9423,7 +9503,7 @@
         <v>0</v>
       </c>
       <c r="H201" s="16" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M201" s="9" t="str" cm="1">
         <f t="array" ref="M201">PAGE_NAME(B201)</f>
@@ -9439,16 +9519,16 @@
         <v>201</v>
       </c>
       <c r="B202" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C202" s="8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D202" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E202" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G202" s="7" t="b">
         <v>0</v>
@@ -9467,10 +9547,10 @@
         <v>202</v>
       </c>
       <c r="B203" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C203" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D203" s="7" t="s">
         <v>29</v>
@@ -9495,10 +9575,10 @@
         <v>203</v>
       </c>
       <c r="B204" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="C204" s="8" t="s">
         <v>296</v>
-      </c>
-      <c r="C204" s="8" t="s">
-        <v>298</v>
       </c>
       <c r="D204" s="7" t="s">
         <v>29</v>
@@ -9523,10 +9603,10 @@
         <v>204</v>
       </c>
       <c r="B205" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C205" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D205" s="7" t="s">
         <v>29</v>
@@ -9551,10 +9631,10 @@
         <v>205</v>
       </c>
       <c r="B206" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C206" s="8" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D206" s="7" t="s">
         <v>29</v>
@@ -9579,10 +9659,10 @@
         <v>206</v>
       </c>
       <c r="B207" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C207" s="8" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D207" s="7" t="s">
         <v>29</v>
@@ -9607,10 +9687,10 @@
         <v>207</v>
       </c>
       <c r="B208" s="11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C208" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D208" s="7" t="s">
         <v>29</v>
@@ -9630,15 +9710,15 @@
         <v/>
       </c>
     </row>
-    <row r="209" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A209" s="7">
         <v>208</v>
       </c>
       <c r="B209" s="11" t="s">
+        <v>300</v>
+      </c>
+      <c r="C209" s="8" t="s">
         <v>302</v>
-      </c>
-      <c r="C209" s="8" t="s">
-        <v>304</v>
       </c>
       <c r="D209" s="7" t="s">
         <v>29</v>
@@ -9658,15 +9738,15 @@
         <v/>
       </c>
     </row>
-    <row r="210" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A210" s="7">
         <v>209</v>
       </c>
       <c r="B210" s="11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C210" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D210" s="7" t="s">
         <v>29</v>
@@ -9686,15 +9766,15 @@
         <v/>
       </c>
     </row>
-    <row r="211" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A211" s="7">
         <v>210</v>
       </c>
       <c r="B211" s="11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C211" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D211" s="7" t="s">
         <v>29</v>
@@ -9714,15 +9794,15 @@
         <v/>
       </c>
     </row>
-    <row r="212" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A212" s="7">
         <v>211</v>
       </c>
       <c r="B212" s="11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C212" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D212" s="7" t="s">
         <v>29</v>
@@ -9742,130 +9822,532 @@
         <v/>
       </c>
     </row>
-    <row r="213" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="M213" s="9" t="str" cm="1">
+    <row r="213" spans="1:20" s="50" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+      <c r="A213" s="7">
+        <v>212</v>
+      </c>
+      <c r="B213" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="C213" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="D213" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E213" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F213" s="8"/>
+      <c r="G213" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H213" s="16"/>
+      <c r="I213" s="30"/>
+      <c r="J213" s="30"/>
+      <c r="K213" s="30"/>
+      <c r="L213" s="30"/>
+      <c r="M213" s="49" t="str" cm="1">
         <f t="array" ref="M213">PAGE_NAME(B213)</f>
-        <v/>
-      </c>
-      <c r="N213" s="9" t="str" cm="1">
+        <v>conformance</v>
+      </c>
+      <c r="N213" s="49" t="str" cm="1">
         <f t="array" ref="N213">SECTION_NAME(B213)</f>
         <v/>
       </c>
-    </row>
-    <row r="214" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="M214" s="9" t="str" cm="1">
+      <c r="O213" s="16"/>
+      <c r="P213" s="16"/>
+      <c r="Q213" s="16"/>
+      <c r="R213" s="16"/>
+      <c r="S213" s="16"/>
+      <c r="T213" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="214" spans="1:20" s="50" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A214" s="7">
+        <v>213</v>
+      </c>
+      <c r="B214" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="C214" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="D214" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E214" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F214" s="8"/>
+      <c r="G214" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H214" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="I214" s="30"/>
+      <c r="J214" s="30"/>
+      <c r="K214" s="30"/>
+      <c r="L214" s="30"/>
+      <c r="M214" s="49" t="str" cm="1">
         <f t="array" ref="M214">PAGE_NAME(B214)</f>
-        <v/>
-      </c>
-      <c r="N214" s="9" t="str" cm="1">
+        <v>conformance</v>
+      </c>
+      <c r="N214" s="49" t="str" cm="1">
         <f t="array" ref="N214">SECTION_NAME(B214)</f>
         <v/>
       </c>
-    </row>
-    <row r="215" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="M215" s="9" t="str" cm="1">
+      <c r="O214" s="16"/>
+      <c r="P214" s="16"/>
+      <c r="Q214" s="16"/>
+      <c r="R214" s="16"/>
+      <c r="S214" s="16"/>
+      <c r="T214" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="215" spans="1:20" s="50" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A215" s="7">
+        <v>214</v>
+      </c>
+      <c r="B215" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="C215" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="D215" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E215" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F215" s="8"/>
+      <c r="G215" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H215" s="16"/>
+      <c r="I215" s="30"/>
+      <c r="J215" s="30"/>
+      <c r="K215" s="30"/>
+      <c r="L215" s="30"/>
+      <c r="M215" s="49" t="str" cm="1">
         <f t="array" ref="M215">PAGE_NAME(B215)</f>
-        <v/>
-      </c>
-      <c r="N215" s="9" t="str" cm="1">
+        <v>conformance</v>
+      </c>
+      <c r="N215" s="49" t="str" cm="1">
         <f t="array" ref="N215">SECTION_NAME(B215)</f>
         <v/>
       </c>
-    </row>
-    <row r="216" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="M216" s="9" t="str" cm="1">
+      <c r="O215" s="16"/>
+      <c r="P215" s="16"/>
+      <c r="Q215" s="16"/>
+      <c r="R215" s="16"/>
+      <c r="S215" s="16"/>
+      <c r="T215" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="216" spans="1:20" s="50" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A216" s="7">
+        <v>215</v>
+      </c>
+      <c r="B216" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="C216" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="D216" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E216" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F216" s="8"/>
+      <c r="G216" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H216" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="I216" s="30"/>
+      <c r="J216" s="30"/>
+      <c r="K216" s="30"/>
+      <c r="L216" s="30"/>
+      <c r="M216" s="49" t="str" cm="1">
         <f t="array" ref="M216">PAGE_NAME(B216)</f>
-        <v/>
-      </c>
-      <c r="N216" s="9" t="str" cm="1">
+        <v>conformance</v>
+      </c>
+      <c r="N216" s="49" t="str" cm="1">
         <f t="array" ref="N216">SECTION_NAME(B216)</f>
         <v/>
       </c>
-    </row>
-    <row r="217" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="M217" s="9" t="str" cm="1">
+      <c r="O216" s="16"/>
+      <c r="P216" s="16"/>
+      <c r="Q216" s="16"/>
+      <c r="R216" s="16"/>
+      <c r="S216" s="16"/>
+      <c r="T216" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="217" spans="1:20" s="50" customFormat="1" ht="272" x14ac:dyDescent="0.2">
+      <c r="A217" s="7">
+        <v>216</v>
+      </c>
+      <c r="B217" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="C217" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="D217" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E217" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F217" s="8"/>
+      <c r="G217" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H217" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="I217" s="30"/>
+      <c r="J217" s="30"/>
+      <c r="K217" s="30"/>
+      <c r="L217" s="30"/>
+      <c r="M217" s="49" t="str" cm="1">
         <f t="array" ref="M217">PAGE_NAME(B217)</f>
-        <v/>
-      </c>
-      <c r="N217" s="9" t="str" cm="1">
+        <v>conformance</v>
+      </c>
+      <c r="N217" s="49" t="str" cm="1">
         <f t="array" ref="N217">SECTION_NAME(B217)</f>
         <v/>
       </c>
-    </row>
-    <row r="218" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="M218" s="9" t="str" cm="1">
+      <c r="O217" s="16"/>
+      <c r="P217" s="16"/>
+      <c r="Q217" s="16"/>
+      <c r="R217" s="16"/>
+      <c r="S217" s="16"/>
+      <c r="T217" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="218" spans="1:20" s="50" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+      <c r="A218" s="7">
+        <v>217</v>
+      </c>
+      <c r="B218" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="C218" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="D218" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E218" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F218" s="8"/>
+      <c r="G218" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H218" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="I218" s="30"/>
+      <c r="J218" s="30"/>
+      <c r="K218" s="30"/>
+      <c r="L218" s="30"/>
+      <c r="M218" s="49" t="str" cm="1">
         <f t="array" ref="M218">PAGE_NAME(B218)</f>
-        <v/>
-      </c>
-      <c r="N218" s="9" t="str" cm="1">
+        <v>conformance</v>
+      </c>
+      <c r="N218" s="49" t="str" cm="1">
         <f t="array" ref="N218">SECTION_NAME(B218)</f>
         <v/>
       </c>
-    </row>
-    <row r="219" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="B219" s="11"/>
-      <c r="M219" s="9" t="str" cm="1">
+      <c r="O218" s="16"/>
+      <c r="P218" s="16"/>
+      <c r="Q218" s="16"/>
+      <c r="R218" s="16"/>
+      <c r="S218" s="16"/>
+      <c r="T218" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="219" spans="1:20" s="50" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+      <c r="A219" s="7">
+        <v>218</v>
+      </c>
+      <c r="B219" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="C219" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="D219" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E219" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F219" s="8"/>
+      <c r="G219" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H219" s="16" t="s">
+        <v>352</v>
+      </c>
+      <c r="I219" s="30"/>
+      <c r="J219" s="30"/>
+      <c r="K219" s="30"/>
+      <c r="L219" s="30"/>
+      <c r="M219" s="49" t="str" cm="1">
         <f t="array" ref="M219">PAGE_NAME(B219)</f>
-        <v/>
-      </c>
-      <c r="N219" s="9" t="str" cm="1">
+        <v>conformance</v>
+      </c>
+      <c r="N219" s="49" t="str" cm="1">
         <f t="array" ref="N219">SECTION_NAME(B219)</f>
         <v/>
       </c>
-    </row>
-    <row r="220" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="B220" s="11"/>
-      <c r="M220" s="9" t="str" cm="1">
+      <c r="O219" s="16"/>
+      <c r="P219" s="16"/>
+      <c r="Q219" s="16"/>
+      <c r="R219" s="16"/>
+      <c r="S219" s="16"/>
+      <c r="T219" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="220" spans="1:20" s="50" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A220" s="7">
+        <v>219</v>
+      </c>
+      <c r="B220" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="C220" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="D220" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E220" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F220" s="8"/>
+      <c r="G220" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H220" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="I220" s="30"/>
+      <c r="J220" s="30"/>
+      <c r="K220" s="30"/>
+      <c r="L220" s="30"/>
+      <c r="M220" s="49" t="str" cm="1">
         <f t="array" ref="M220">PAGE_NAME(B220)</f>
-        <v/>
-      </c>
-      <c r="N220" s="9" t="str" cm="1">
+        <v>conformance</v>
+      </c>
+      <c r="N220" s="49" t="str" cm="1">
         <f t="array" ref="N220">SECTION_NAME(B220)</f>
         <v/>
       </c>
-    </row>
-    <row r="221" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="B221" s="11"/>
-      <c r="M221" s="9" t="str" cm="1">
+      <c r="O220" s="16"/>
+      <c r="P220" s="16"/>
+      <c r="Q220" s="16"/>
+      <c r="R220" s="16"/>
+      <c r="S220" s="16"/>
+      <c r="T220" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="221" spans="1:20" s="50" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A221" s="7">
+        <v>220</v>
+      </c>
+      <c r="B221" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="C221" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="D221" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E221" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F221" s="8"/>
+      <c r="G221" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H221" s="16"/>
+      <c r="I221" s="30"/>
+      <c r="J221" s="30"/>
+      <c r="K221" s="30"/>
+      <c r="L221" s="30"/>
+      <c r="M221" s="49" t="str" cm="1">
         <f t="array" ref="M221">PAGE_NAME(B221)</f>
-        <v/>
-      </c>
-      <c r="N221" s="9" t="str" cm="1">
+        <v>conformance</v>
+      </c>
+      <c r="N221" s="49" t="str" cm="1">
         <f t="array" ref="N221">SECTION_NAME(B221)</f>
         <v/>
       </c>
-    </row>
-    <row r="222" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="B222" s="11"/>
-      <c r="M222" s="9" t="str" cm="1">
+      <c r="O221" s="16"/>
+      <c r="P221" s="16"/>
+      <c r="Q221" s="16"/>
+      <c r="R221" s="16"/>
+      <c r="S221" s="16"/>
+      <c r="T221" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="222" spans="1:20" s="50" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A222" s="7">
+        <v>221</v>
+      </c>
+      <c r="B222" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="C222" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="D222" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E222" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F222" s="8"/>
+      <c r="G222" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H222" s="16" t="s">
+        <v>357</v>
+      </c>
+      <c r="I222" s="30"/>
+      <c r="J222" s="30"/>
+      <c r="K222" s="30"/>
+      <c r="L222" s="30"/>
+      <c r="M222" s="49" t="str" cm="1">
         <f t="array" ref="M222">PAGE_NAME(B222)</f>
-        <v/>
-      </c>
-      <c r="N222" s="9" t="str" cm="1">
+        <v>conformance</v>
+      </c>
+      <c r="N222" s="49" t="str" cm="1">
         <f t="array" ref="N222">SECTION_NAME(B222)</f>
         <v/>
       </c>
-    </row>
-    <row r="223" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="B223" s="11"/>
-      <c r="M223" s="9" t="str" cm="1">
+      <c r="O222" s="16"/>
+      <c r="P222" s="16"/>
+      <c r="Q222" s="16"/>
+      <c r="R222" s="16"/>
+      <c r="S222" s="16"/>
+      <c r="T222" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="223" spans="1:20" s="50" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A223" s="7">
+        <v>222</v>
+      </c>
+      <c r="B223" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="C223" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="D223" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E223" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F223" s="8"/>
+      <c r="G223" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H223" s="16" t="s">
+        <v>359</v>
+      </c>
+      <c r="I223" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="J223" s="30" t="s">
+        <v>360</v>
+      </c>
+      <c r="K223" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="L223" s="30"/>
+      <c r="M223" s="49" t="str" cm="1">
         <f t="array" ref="M223">PAGE_NAME(B223)</f>
-        <v/>
-      </c>
-      <c r="N223" s="9" t="str" cm="1">
+        <v>conformance</v>
+      </c>
+      <c r="N223" s="49" t="str" cm="1">
         <f t="array" ref="N223">SECTION_NAME(B223)</f>
         <v/>
       </c>
-    </row>
-    <row r="224" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="B224" s="11"/>
-      <c r="M224" s="9" t="str" cm="1">
+      <c r="O223" s="16"/>
+      <c r="P223" s="16"/>
+      <c r="Q223" s="16"/>
+      <c r="R223" s="16"/>
+      <c r="S223" s="16"/>
+      <c r="T223" s="16" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="224" spans="1:20" s="50" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+      <c r="A224" s="7">
+        <v>223</v>
+      </c>
+      <c r="B224" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="C224" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="D224" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E224" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F224" s="8"/>
+      <c r="G224" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H224" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="I224" s="30"/>
+      <c r="J224" s="30"/>
+      <c r="K224" s="30"/>
+      <c r="L224" s="30"/>
+      <c r="M224" s="49" t="str" cm="1">
         <f t="array" ref="M224">PAGE_NAME(B224)</f>
-        <v/>
-      </c>
-      <c r="N224" s="9" t="str" cm="1">
+        <v>conformance</v>
+      </c>
+      <c r="N224" s="49" t="str" cm="1">
         <f t="array" ref="N224">SECTION_NAME(B224)</f>
         <v/>
+      </c>
+      <c r="O224" s="16"/>
+      <c r="P224" s="16"/>
+      <c r="Q224" s="16"/>
+      <c r="R224" s="16"/>
+      <c r="S224" s="16"/>
+      <c r="T224" s="16" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="225" spans="2:14" ht="16" x14ac:dyDescent="0.2">
@@ -11114,6 +11596,9 @@
     <hyperlink ref="B188" r:id="rId61" xr:uid="{0CF8476F-3EB0-4E4F-8427-B5593D7E7445}"/>
     <hyperlink ref="B160" r:id="rId62" location="updating-authorization-requests" xr:uid="{3D5A271C-1C5A-174B-BFE7-B13D790828C2}"/>
     <hyperlink ref="B84" r:id="rId63" location="prior-authorization-submission" xr:uid="{AC29C7DD-97E9-3944-AB1F-49A4A8ED6F5A}"/>
+    <hyperlink ref="B213" r:id="rId64" xr:uid="{94CD23A1-97BD-7B40-B486-86E941073FD1}"/>
+    <hyperlink ref="B214:B224" r:id="rId65" display="https://hl7.org/fhir/us/davinci-hrex/STU1/conformance.html" xr:uid="{E34E44FA-11CF-BE4D-AF14-8EE2BC19BC3D}"/>
+    <hyperlink ref="B220" r:id="rId66" xr:uid="{DB18FEC9-17CA-2E4C-8CE6-F72A11DD3204}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -11123,19 +11608,19 @@
           <x14:formula1>
             <xm:f>'Column Data'!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G1048576</xm:sqref>
+          <xm:sqref>G1:G212 G225:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4866B9BF-5615-6646-965F-909D4D65F2A5}">
           <x14:formula1>
             <xm:f>'Column Data'!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>D2:D212 D225:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F4FB27A2-804E-CB49-B85C-BBEE0C688B4F}">
           <x14:formula1>
             <xm:f>'Column Data'!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1048576 I2:I1048576</xm:sqref>
+          <xm:sqref>I225:I1048576 I2:I212 K2:K212 K225:K1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -11159,7 +11644,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="48" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B1" s="48"/>
     </row>
@@ -11169,82 +11654,82 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="136" x14ac:dyDescent="0.2">
       <c r="B15" s="41" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -11275,19 +11760,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>326</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>327</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>328</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -11295,13 +11780,13 @@
         <v>0.1</v>
       </c>
       <c r="B2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D2" t="s">
         <v>330</v>
-      </c>
-      <c r="C2" t="s">
-        <v>331</v>
-      </c>
-      <c r="D2" t="s">
-        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -11321,13 +11806,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D1" t="s">
         <v>15</v>
@@ -11341,7 +11826,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D2" t="s">
         <v>55</v>
@@ -11355,7 +11840,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>
@@ -11366,7 +11851,7 @@
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -11376,12 +11861,12 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -11390,6 +11875,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC335ED7BB179244BF94A0DFE64544DC" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3a0f66abe5d2a0564332877ab55d3f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eebd8b74-b9de-41b2-9247-c010c4973c2b" xmlns:ns3="b7009bbd-f938-489b-a530-f05273710fff" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ec7ca2ee893ff8a0f61d4046c6461645" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
@@ -11643,19 +12141,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -11666,6 +12151,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
+    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12FB330C-B068-4EE3-928A-A72A297ABA91}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11685,24 +12188,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
-    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
   <ds:schemaRefs>

</xml_diff>